<commit_message>
Fixed issue #13 Permitir que en los ficheros de metadatos dos columnas se puedan relacionar para crear SKOS jerárquicos
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010007-A-TC-TM-TP.xlsx
+++ b/data/metadata/Informe-01-010007-A-TC-TM-TP.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Comarca nombre</t>
   </si>
@@ -38,6 +38,33 @@
   </si>
   <si>
     <t>Municipio nombre</t>
+  </si>
+  <si>
+    <t>comarca-nombre</t>
+  </si>
+  <si>
+    <t>refrigeracion</t>
+  </si>
+  <si>
+    <t>numero-hogares</t>
+  </si>
+  <si>
+    <t>comarca-codigo</t>
+  </si>
+  <si>
+    <t>provincia-codigo</t>
+  </si>
+  <si>
+    <t>aragon</t>
+  </si>
+  <si>
+    <t>municipio-codigo</t>
+  </si>
+  <si>
+    <t>provincia-nombre</t>
+  </si>
+  <si>
+    <t>municipio-nombre</t>
   </si>
   <si>
     <t>sdmx-dimension:refArea</t>
@@ -179,82 +206,111 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>